<commit_message>
Added bom, production, unit and currency ontology.
</commit_message>
<xml_diff>
--- a/ontology/ontology_tables/encoding_ontology.xlsx
+++ b/ontology/ontology_tables/encoding_ontology.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/q436477/Projekte/knowledge_agents/ontology/ontology_tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF4513D-019A-9E43-A04B-70F5E2B9271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-1380" yWindow="-21100" windowWidth="31340" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
   <si>
     <t>type</t>
   </si>
@@ -185,9 +191,6 @@
   </si>
   <si>
     <t>xsd:integer</t>
-  </si>
-  <si>
-    <t>owl:Thing</t>
   </si>
   <si>
     <t>Encodierung</t>
@@ -337,8 +340,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,14 +419,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
       <font>
-        <b/>
-        <color rgb="FF0000FF"/>
+        <color rgb="FF800080"/>
       </font>
     </dxf>
     <dxf>
@@ -433,16 +435,25 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF800080"/>
+        <b/>
+        <color rgb="FF0000FF"/>
       </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,7 +495,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,9 +527,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,6 +579,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -725,17 +772,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="16.5703125" style="1" customWidth="1"/>
+    <col min="1" max="13" width="16.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -776,7 +825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -784,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -792,7 +841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -800,7 +849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -808,7 +857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -816,12 +865,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -829,12 +878,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -845,19 +894,19 @@
         <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -871,7 +920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -885,7 +934,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -899,13 +948,13 @@
         <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -919,16 +968,16 @@
         <v>55</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -942,13 +991,13 @@
         <v>55</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -962,16 +1011,16 @@
         <v>56</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="1">
         <v>17</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -985,13 +1034,13 @@
         <v>56</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1005,16 +1054,16 @@
         <v>55</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1025,16 +1074,16 @@
         <v>54</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1044,17 +1093,14 @@
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1068,16 +1114,16 @@
         <v>56</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1091,13 +1137,13 @@
         <v>55</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1108,13 +1154,13 @@
         <v>39</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1128,19 +1174,19 @@
         <v>56</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -1151,13 +1197,13 @@
         <v>39</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1171,13 +1217,13 @@
         <v>56</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1191,13 +1237,13 @@
         <v>56</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -1211,13 +1257,13 @@
         <v>56</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1228,13 +1274,13 @@
         <v>54</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -1248,13 +1294,13 @@
         <v>39</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>22</v>
       </c>
@@ -1268,10 +1314,10 @@
         <v>49</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,16 +1331,16 @@
         <v>55</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -1308,32 +1354,32 @@
         <v>55</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A999">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"relation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"attribute"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location=""/>
-    <hyperlink ref="M12" r:id="rId2"/>
-    <hyperlink ref="M20" r:id="rId3"/>
-    <hyperlink ref="M22" r:id="rId4" location="Tokenization"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M22" r:id="rId4" location="Tokenization" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>